<commit_message>
slice analysis some qpcr expermients
</commit_message>
<xml_diff>
--- a/StepOnePlusData/platelayoutreagents.xlsx
+++ b/StepOnePlusData/platelayoutreagents.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="114">
   <si>
     <t>h20</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>Total volume</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>primer</t>
+  </si>
+  <si>
+    <t>Enzyme mix</t>
   </si>
 </sst>
 </file>
@@ -597,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -704,7 +713,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -714,9 +733,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,9 +776,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,21 +1057,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z85"/>
+  <dimension ref="A1:Z108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75:AA84"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
     <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="2" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" customWidth="1"/>
     <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.85546875" customWidth="1"/>
     <col min="22" max="22" width="9.42578125" customWidth="1"/>
@@ -1132,26 +1147,26 @@
       <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63" t="s">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1167,26 +1182,26 @@
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="F3" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63" t="s">
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63" t="s">
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63" t="s">
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
       <c r="R3" s="25">
         <v>42167</v>
       </c>
@@ -1205,26 +1220,26 @@
       <c r="E4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63" t="s">
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63" t="s">
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
       <c r="R4" s="27" t="s">
         <v>67</v>
       </c>
@@ -1243,26 +1258,26 @@
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63" t="s">
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63" t="s">
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63" t="s">
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1278,26 +1293,26 @@
       <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="63" t="s">
+      <c r="F6" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63" t="s">
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63" t="s">
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63" t="s">
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1313,18 +1328,18 @@
       <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1337,18 +1352,18 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1412,26 +1427,26 @@
       <c r="E10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="61" t="s">
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="64" t="s">
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="61" t="s">
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="67"/>
       <c r="R10" s="25">
         <v>42177</v>
       </c>
@@ -1440,26 +1455,26 @@
       <c r="E11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="61" t="s">
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="64" t="s">
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="61" t="s">
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
       <c r="R11" s="28" t="s">
         <v>68</v>
       </c>
@@ -1476,26 +1491,26 @@
       <c r="E12" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="61" t="s">
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="64" t="s">
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="61" t="s">
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
       <c r="R12" s="29" t="s">
         <v>69</v>
       </c>
@@ -1514,26 +1529,26 @@
       <c r="E13" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="61" t="s">
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="64" t="s">
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="61" t="s">
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1549,26 +1564,26 @@
       <c r="E14" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="61" t="s">
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="64" t="s">
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="61" t="s">
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1584,26 +1599,26 @@
       <c r="E15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="61" t="s">
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="64" t="s">
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="61" t="s">
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1619,26 +1634,26 @@
       <c r="E16" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="61" t="s">
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="64" t="s">
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="61" t="s">
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -1650,26 +1665,26 @@
       <c r="E17" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="61" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="64" t="s">
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="61" t="s">
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E19" s="38"/>
@@ -1721,26 +1736,26 @@
       <c r="E20" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="61" t="s">
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="64" t="s">
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="61" t="s">
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
       <c r="R20" s="25">
         <v>42177</v>
       </c>
@@ -1756,26 +1771,26 @@
       <c r="E21" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="64" t="s">
+      <c r="F21" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="61" t="s">
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="64" t="s">
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="61" t="s">
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
       <c r="R21" s="28" t="s">
         <v>68</v>
       </c>
@@ -1794,26 +1809,26 @@
       <c r="E22" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="61" t="s">
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="64" t="s">
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="61" t="s">
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="61"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
       <c r="R22" s="29" t="s">
         <v>69</v>
       </c>
@@ -1832,18 +1847,18 @@
       <c r="E23" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1920,27 +1935,27 @@
       <c r="E26" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="65" t="str">
+      <c r="F26" s="70" t="str">
         <f>"1:2"</f>
         <v>1:2</v>
       </c>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66" t="str">
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="71" t="str">
         <f t="shared" ref="I26" si="3">"1:2"</f>
         <v>1:2</v>
       </c>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="67" t="str">
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="72" t="str">
         <f t="shared" ref="L26" si="4">"1:2"</f>
         <v>1:2</v>
       </c>
-      <c r="M26" s="67"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
       <c r="R26" s="25">
         <v>42178</v>
       </c>
@@ -1959,27 +1974,27 @@
       <c r="E27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="65" t="str">
+      <c r="F27" s="70" t="str">
         <f>"1:4"</f>
         <v>1:4</v>
       </c>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66" t="str">
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71" t="str">
         <f t="shared" ref="I27" si="5">"1:4"</f>
         <v>1:4</v>
       </c>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="67" t="str">
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="72" t="str">
         <f t="shared" ref="L27" si="6">"1:4"</f>
         <v>1:4</v>
       </c>
-      <c r="M27" s="67"/>
-      <c r="N27" s="67"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="60"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
       <c r="R27" s="16" t="s">
         <v>42</v>
       </c>
@@ -1998,27 +2013,27 @@
       <c r="E28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="65" t="str">
+      <c r="F28" s="70" t="str">
         <f>"1:8"</f>
         <v>1:8</v>
       </c>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="66" t="str">
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71" t="str">
         <f t="shared" ref="I28" si="7">"1:8"</f>
         <v>1:8</v>
       </c>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="67" t="str">
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="72" t="str">
         <f t="shared" ref="L28" si="8">"1:8"</f>
         <v>1:8</v>
       </c>
-      <c r="M28" s="67"/>
-      <c r="N28" s="67"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
       <c r="R28" s="15" t="s">
         <v>43</v>
       </c>
@@ -2036,27 +2051,27 @@
       <c r="E29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="65" t="str">
+      <c r="F29" s="70" t="str">
         <f>"1:16"</f>
         <v>1:16</v>
       </c>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="66" t="str">
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="71" t="str">
         <f t="shared" ref="I29" si="9">"1:16"</f>
         <v>1:16</v>
       </c>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="67" t="str">
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="72" t="str">
         <f t="shared" ref="L29" si="10">"1:16"</f>
         <v>1:16</v>
       </c>
-      <c r="M29" s="67"/>
-      <c r="N29" s="67"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
       <c r="R29" s="14" t="s">
         <v>44</v>
       </c>
@@ -2065,27 +2080,27 @@
       <c r="E30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="65" t="str">
+      <c r="F30" s="70" t="str">
         <f>"1:32"</f>
         <v>1:32</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="66" t="str">
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71" t="str">
         <f t="shared" ref="I30" si="11">"1:32"</f>
         <v>1:32</v>
       </c>
-      <c r="J30" s="66"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="67" t="str">
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="72" t="str">
         <f t="shared" ref="L30" si="12">"1:32"</f>
         <v>1:32</v>
       </c>
-      <c r="M30" s="67"/>
-      <c r="N30" s="67"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
@@ -2098,29 +2113,29 @@
       <c r="E31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="65" t="str">
+      <c r="F31" s="70" t="str">
         <f>"1:64"</f>
         <v>1:64</v>
       </c>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66" t="str">
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71" t="str">
         <f t="shared" ref="I31" si="13">"1:64"</f>
         <v>1:64</v>
       </c>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="67" t="str">
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="72" t="str">
         <f t="shared" ref="L31" si="14">"1:64"</f>
         <v>1:64</v>
       </c>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="65" t="s">
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="65"/>
+      <c r="P31" s="70"/>
+      <c r="Q31" s="70"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2136,29 +2151,29 @@
       <c r="E32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="65" t="str">
+      <c r="F32" s="70" t="str">
         <f>"1:128"</f>
         <v>1:128</v>
       </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="66" t="str">
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71" t="str">
         <f t="shared" ref="I32" si="15">"1:128"</f>
         <v>1:128</v>
       </c>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="67" t="str">
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="72" t="str">
         <f t="shared" ref="L32" si="16">"1:128"</f>
         <v>1:128</v>
       </c>
-      <c r="M32" s="67"/>
-      <c r="N32" s="67"/>
-      <c r="O32" s="66" t="s">
+      <c r="M32" s="72"/>
+      <c r="N32" s="72"/>
+      <c r="O32" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="P32" s="66"/>
-      <c r="Q32" s="66"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2174,29 +2189,29 @@
       <c r="E33" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="65" t="str">
+      <c r="F33" s="70" t="str">
         <f>"1:256"</f>
         <v>1:256</v>
       </c>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66" t="str">
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="71" t="str">
         <f t="shared" ref="I33" si="18">"1:256"</f>
         <v>1:256</v>
       </c>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="67" t="str">
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="72" t="str">
         <f t="shared" ref="L33" si="19">"1:256"</f>
         <v>1:256</v>
       </c>
-      <c r="M33" s="67"/>
-      <c r="N33" s="67"/>
-      <c r="O33" s="67" t="s">
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="67"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="72"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -2278,24 +2293,24 @@
       <c r="E37" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="61" t="s">
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="63" t="s">
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="M37" s="63"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="60"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="65"/>
+      <c r="P37" s="65"/>
+      <c r="Q37" s="65"/>
       <c r="R37" s="25">
         <v>42183</v>
       </c>
@@ -2314,24 +2329,24 @@
       <c r="E38" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="64" t="s">
+      <c r="F38" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="61" t="s">
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="63" t="s">
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="M38" s="63"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="60"/>
-      <c r="P38" s="60"/>
-      <c r="Q38" s="60"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="65"/>
+      <c r="Q38" s="65"/>
       <c r="R38" s="28" t="s">
         <v>68</v>
       </c>
@@ -2357,24 +2372,24 @@
       <c r="E39" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="64" t="s">
+      <c r="F39" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="61" t="s">
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="63" t="s">
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="M39" s="63"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="60"/>
-      <c r="Q39" s="60"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="65"/>
+      <c r="P39" s="65"/>
+      <c r="Q39" s="65"/>
       <c r="R39" s="29" t="s">
         <v>69</v>
       </c>
@@ -2400,24 +2415,24 @@
       <c r="E40" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="64" t="s">
+      <c r="F40" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="61" t="s">
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="63" t="s">
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="M40" s="63"/>
-      <c r="N40" s="63"/>
-      <c r="O40" s="60"/>
-      <c r="P40" s="60"/>
-      <c r="Q40" s="60"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="65"/>
+      <c r="P40" s="65"/>
+      <c r="Q40" s="65"/>
       <c r="R40" s="27" t="s">
         <v>67</v>
       </c>
@@ -2446,24 +2461,24 @@
       <c r="E41" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="61" t="s">
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="63" t="s">
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="M41" s="63"/>
-      <c r="N41" s="63"/>
-      <c r="O41" s="60"/>
-      <c r="P41" s="60"/>
-      <c r="Q41" s="60"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="65"/>
+      <c r="P41" s="65"/>
+      <c r="Q41" s="65"/>
       <c r="R41" s="46" t="s">
         <v>82</v>
       </c>
@@ -2488,24 +2503,24 @@
       <c r="E42" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="64" t="s">
+      <c r="F42" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="61" t="s">
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="63" t="s">
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="60"/>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="60"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="69"/>
+      <c r="O42" s="65"/>
+      <c r="P42" s="65"/>
+      <c r="Q42" s="65"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -2521,24 +2536,24 @@
       <c r="E43" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="64" t="s">
+      <c r="F43" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="61" t="s">
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="63" t="s">
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="60"/>
-      <c r="Q43" s="60"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -2554,24 +2569,24 @@
       <c r="E44" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="61" t="s">
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="63" t="s">
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="M44" s="63"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="60"/>
-      <c r="P44" s="60"/>
-      <c r="Q44" s="60"/>
+      <c r="M44" s="69"/>
+      <c r="N44" s="69"/>
+      <c r="O44" s="65"/>
+      <c r="P44" s="65"/>
+      <c r="Q44" s="65"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -2648,24 +2663,24 @@
       <c r="E47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="64" t="s">
+      <c r="F47" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="61" t="s">
+      <c r="G47" s="66"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J47" s="61"/>
-      <c r="K47" s="61"/>
-      <c r="L47" s="63" t="s">
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="60"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="65"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="65"/>
       <c r="R47" s="25" t="s">
         <v>83</v>
       </c>
@@ -2683,24 +2698,24 @@
       <c r="E48" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="64" t="s">
+      <c r="F48" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="61" t="s">
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="63" t="s">
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="60"/>
-      <c r="P48" s="60"/>
-      <c r="Q48" s="60"/>
+      <c r="M48" s="69"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="65"/>
+      <c r="P48" s="65"/>
+      <c r="Q48" s="65"/>
       <c r="R48" s="28" t="s">
         <v>68</v>
       </c>
@@ -2709,24 +2724,24 @@
       <c r="E49" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="64" t="s">
+      <c r="F49" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="61" t="s">
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="63" t="s">
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="60"/>
-      <c r="Q49" s="60"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65"/>
+      <c r="Q49" s="65"/>
       <c r="R49" s="29" t="s">
         <v>69</v>
       </c>
@@ -2735,24 +2750,24 @@
       <c r="E50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="64" t="s">
+      <c r="F50" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="61" t="s">
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="63" t="s">
+      <c r="J50" s="67"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="60"/>
-      <c r="Q50" s="60"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="65"/>
+      <c r="P50" s="65"/>
+      <c r="Q50" s="65"/>
       <c r="R50" s="27" t="s">
         <v>67</v>
       </c>
@@ -2761,93 +2776,93 @@
       <c r="E51" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="64" t="s">
+      <c r="F51" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="61" t="s">
+      <c r="G51" s="66"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="J51" s="61"/>
-      <c r="K51" s="61"/>
-      <c r="L51" s="63" t="s">
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="M51" s="63"/>
-      <c r="N51" s="63"/>
-      <c r="O51" s="60"/>
-      <c r="P51" s="60"/>
-      <c r="Q51" s="60"/>
+      <c r="M51" s="69"/>
+      <c r="N51" s="69"/>
+      <c r="O51" s="65"/>
+      <c r="P51" s="65"/>
+      <c r="Q51" s="65"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E52" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="64" t="s">
+      <c r="F52" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="61" t="s">
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="J52" s="61"/>
-      <c r="K52" s="61"/>
-      <c r="L52" s="63" t="s">
+      <c r="J52" s="67"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="M52" s="63"/>
-      <c r="N52" s="63"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="60"/>
+      <c r="M52" s="69"/>
+      <c r="N52" s="69"/>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E53" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="64" t="s">
+      <c r="F53" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="61" t="s">
+      <c r="G53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="J53" s="61"/>
-      <c r="K53" s="61"/>
-      <c r="L53" s="63" t="s">
+      <c r="J53" s="67"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="M53" s="63"/>
-      <c r="N53" s="63"/>
-      <c r="O53" s="60"/>
-      <c r="P53" s="60"/>
-      <c r="Q53" s="60"/>
+      <c r="M53" s="69"/>
+      <c r="N53" s="69"/>
+      <c r="O53" s="65"/>
+      <c r="P53" s="65"/>
+      <c r="Q53" s="65"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E54" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="64" t="s">
+      <c r="F54" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="61" t="s">
+      <c r="G54" s="66"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="J54" s="61"/>
-      <c r="K54" s="61"/>
-      <c r="L54" s="63" t="s">
+      <c r="J54" s="67"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="M54" s="63"/>
-      <c r="N54" s="63"/>
-      <c r="O54" s="60"/>
-      <c r="P54" s="60"/>
-      <c r="Q54" s="60"/>
+      <c r="M54" s="69"/>
+      <c r="N54" s="69"/>
+      <c r="O54" s="65"/>
+      <c r="P54" s="65"/>
+      <c r="Q54" s="65"/>
     </row>
     <row r="55" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="35"/>
@@ -2906,24 +2921,24 @@
       <c r="E57" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F57" s="68" t="s">
+      <c r="F57" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="G57" s="69"/>
-      <c r="H57" s="70"/>
-      <c r="I57" s="71" t="s">
+      <c r="G57" s="74"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="J57" s="72"/>
-      <c r="K57" s="73"/>
-      <c r="L57" s="74" t="s">
+      <c r="J57" s="77"/>
+      <c r="K57" s="78"/>
+      <c r="L57" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="M57" s="75"/>
-      <c r="N57" s="76"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
+      <c r="M57" s="80"/>
+      <c r="N57" s="81"/>
+      <c r="O57" s="65"/>
+      <c r="P57" s="65"/>
+      <c r="Q57" s="65"/>
       <c r="R57" s="25" t="s">
         <v>83</v>
       </c>
@@ -2932,24 +2947,24 @@
       <c r="E58" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="68" t="s">
+      <c r="F58" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="G58" s="69"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="71" t="s">
+      <c r="G58" s="74"/>
+      <c r="H58" s="75"/>
+      <c r="I58" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="J58" s="72"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="74" t="s">
+      <c r="J58" s="77"/>
+      <c r="K58" s="78"/>
+      <c r="L58" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="M58" s="75"/>
-      <c r="N58" s="76"/>
-      <c r="O58" s="60"/>
-      <c r="P58" s="60"/>
-      <c r="Q58" s="60"/>
+      <c r="M58" s="80"/>
+      <c r="N58" s="81"/>
+      <c r="O58" s="65"/>
+      <c r="P58" s="65"/>
+      <c r="Q58" s="65"/>
       <c r="R58" s="28" t="s">
         <v>68</v>
       </c>
@@ -2958,24 +2973,24 @@
       <c r="E59" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="68" t="s">
+      <c r="F59" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="G59" s="69"/>
-      <c r="H59" s="70"/>
-      <c r="I59" s="71" t="s">
+      <c r="G59" s="74"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="J59" s="72"/>
-      <c r="K59" s="73"/>
-      <c r="L59" s="74" t="s">
+      <c r="J59" s="77"/>
+      <c r="K59" s="78"/>
+      <c r="L59" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="M59" s="75"/>
-      <c r="N59" s="76"/>
-      <c r="O59" s="60"/>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="60"/>
+      <c r="M59" s="80"/>
+      <c r="N59" s="81"/>
+      <c r="O59" s="65"/>
+      <c r="P59" s="65"/>
+      <c r="Q59" s="65"/>
       <c r="R59" s="29" t="s">
         <v>69</v>
       </c>
@@ -2984,24 +2999,24 @@
       <c r="E60" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="68" t="s">
+      <c r="F60" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="G60" s="69"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="71" t="s">
+      <c r="G60" s="74"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="J60" s="72"/>
-      <c r="K60" s="73"/>
-      <c r="L60" s="74" t="s">
+      <c r="J60" s="77"/>
+      <c r="K60" s="78"/>
+      <c r="L60" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="M60" s="75"/>
-      <c r="N60" s="76"/>
-      <c r="O60" s="60"/>
-      <c r="P60" s="60"/>
-      <c r="Q60" s="60"/>
+      <c r="M60" s="80"/>
+      <c r="N60" s="81"/>
+      <c r="O60" s="65"/>
+      <c r="P60" s="65"/>
+      <c r="Q60" s="65"/>
       <c r="R60" s="27" t="s">
         <v>67</v>
       </c>
@@ -3010,41 +3025,41 @@
       <c r="E61" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="68" t="s">
+      <c r="F61" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G61" s="69"/>
-      <c r="H61" s="70"/>
-      <c r="I61" s="71" t="s">
+      <c r="G61" s="74"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="J61" s="72"/>
-      <c r="K61" s="73"/>
-      <c r="L61" s="74" t="s">
+      <c r="J61" s="77"/>
+      <c r="K61" s="78"/>
+      <c r="L61" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="M61" s="75"/>
-      <c r="N61" s="76"/>
-      <c r="O61" s="60"/>
-      <c r="P61" s="60"/>
-      <c r="Q61" s="60"/>
+      <c r="M61" s="80"/>
+      <c r="N61" s="81"/>
+      <c r="O61" s="65"/>
+      <c r="P61" s="65"/>
+      <c r="Q61" s="65"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E62" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="60"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="60"/>
-      <c r="J62" s="60"/>
-      <c r="K62" s="60"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-      <c r="O62" s="60"/>
-      <c r="P62" s="60"/>
-      <c r="Q62" s="60"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="65"/>
+      <c r="J62" s="65"/>
+      <c r="K62" s="65"/>
+      <c r="L62" s="65"/>
+      <c r="M62" s="65"/>
+      <c r="N62" s="65"/>
+      <c r="O62" s="65"/>
+      <c r="P62" s="65"/>
+      <c r="Q62" s="65"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
@@ -3375,12 +3390,12 @@
         <v>74</v>
       </c>
       <c r="K70" s="49"/>
-      <c r="L70" s="77"/>
-      <c r="M70" s="78"/>
-      <c r="N70" s="77"/>
-      <c r="O70" s="78"/>
-      <c r="P70" s="77"/>
-      <c r="Q70" s="78"/>
+      <c r="L70" s="82"/>
+      <c r="M70" s="83"/>
+      <c r="N70" s="82"/>
+      <c r="O70" s="83"/>
+      <c r="P70" s="82"/>
+      <c r="Q70" s="83"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
@@ -3408,12 +3423,12 @@
         <v>75</v>
       </c>
       <c r="K71" s="49"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="78"/>
-      <c r="N71" s="77"/>
-      <c r="O71" s="78"/>
-      <c r="P71" s="77"/>
-      <c r="Q71" s="78"/>
+      <c r="L71" s="82"/>
+      <c r="M71" s="83"/>
+      <c r="N71" s="82"/>
+      <c r="O71" s="83"/>
+      <c r="P71" s="82"/>
+      <c r="Q71" s="83"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -3441,12 +3456,12 @@
         <v>76</v>
       </c>
       <c r="K72" s="49"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="78"/>
-      <c r="N72" s="77"/>
-      <c r="O72" s="78"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="78"/>
+      <c r="L72" s="82"/>
+      <c r="M72" s="83"/>
+      <c r="N72" s="82"/>
+      <c r="O72" s="83"/>
+      <c r="P72" s="82"/>
+      <c r="Q72" s="83"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
@@ -3460,10 +3475,26 @@
       </c>
     </row>
     <row r="75" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="V75" s="79" t="s">
+      <c r="E75" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="46"/>
+      <c r="I75" s="46"/>
+      <c r="J75" s="46"/>
+      <c r="K75" s="46"/>
+      <c r="L75" s="46"/>
+      <c r="M75" s="46"/>
+      <c r="N75" s="46"/>
+      <c r="O75" s="46"/>
+      <c r="P75" s="46"/>
+      <c r="Q75" s="46"/>
+      <c r="R75" s="46"/>
+      <c r="V75" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="W75" s="79"/>
+      <c r="W75" s="60"/>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
@@ -3540,26 +3571,26 @@
       <c r="E77" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F77" s="64" t="s">
+      <c r="F77" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="G77" s="64"/>
-      <c r="H77" s="64"/>
-      <c r="I77" s="61" t="s">
+      <c r="G77" s="66"/>
+      <c r="H77" s="66"/>
+      <c r="I77" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="J77" s="61"/>
-      <c r="K77" s="61"/>
-      <c r="L77" s="64" t="s">
+      <c r="J77" s="67"/>
+      <c r="K77" s="67"/>
+      <c r="L77" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="M77" s="64"/>
-      <c r="N77" s="64"/>
-      <c r="O77" s="61" t="s">
+      <c r="M77" s="66"/>
+      <c r="N77" s="66"/>
+      <c r="O77" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="P77" s="61"/>
-      <c r="Q77" s="61"/>
+      <c r="P77" s="67"/>
+      <c r="Q77" s="67"/>
       <c r="R77" s="25">
         <v>42248</v>
       </c>
@@ -3598,22 +3629,22 @@
       <c r="E78" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="64" t="s">
+      <c r="F78" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="G78" s="64"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="61" t="s">
+      <c r="G78" s="66"/>
+      <c r="H78" s="66"/>
+      <c r="I78" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="J78" s="61"/>
-      <c r="K78" s="61"/>
-      <c r="L78" s="60"/>
-      <c r="M78" s="60"/>
-      <c r="N78" s="60"/>
-      <c r="O78" s="60"/>
-      <c r="P78" s="60"/>
-      <c r="Q78" s="60"/>
+      <c r="J78" s="67"/>
+      <c r="K78" s="67"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="65"/>
+      <c r="N78" s="65"/>
+      <c r="O78" s="65"/>
+      <c r="P78" s="65"/>
+      <c r="Q78" s="65"/>
       <c r="R78" s="28" t="s">
         <v>107</v>
       </c>
@@ -3652,22 +3683,22 @@
       <c r="E79" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="64" t="s">
+      <c r="F79" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="G79" s="64"/>
-      <c r="H79" s="64"/>
-      <c r="I79" s="61" t="s">
+      <c r="G79" s="66"/>
+      <c r="H79" s="66"/>
+      <c r="I79" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="J79" s="61"/>
-      <c r="K79" s="61"/>
-      <c r="L79" s="60"/>
-      <c r="M79" s="60"/>
-      <c r="N79" s="60"/>
-      <c r="O79" s="60"/>
-      <c r="P79" s="60"/>
-      <c r="Q79" s="60"/>
+      <c r="J79" s="67"/>
+      <c r="K79" s="67"/>
+      <c r="L79" s="65"/>
+      <c r="M79" s="65"/>
+      <c r="N79" s="65"/>
+      <c r="O79" s="65"/>
+      <c r="P79" s="65"/>
+      <c r="Q79" s="65"/>
       <c r="R79" s="29" t="s">
         <v>108</v>
       </c>
@@ -3706,22 +3737,22 @@
       <c r="E80" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F80" s="64" t="s">
+      <c r="F80" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="G80" s="64"/>
-      <c r="H80" s="64"/>
-      <c r="I80" s="61" t="s">
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
+      <c r="I80" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="J80" s="61"/>
-      <c r="K80" s="61"/>
-      <c r="L80" s="60"/>
-      <c r="M80" s="60"/>
-      <c r="N80" s="60"/>
-      <c r="O80" s="60"/>
-      <c r="P80" s="60"/>
-      <c r="Q80" s="60"/>
+      <c r="J80" s="67"/>
+      <c r="K80" s="67"/>
+      <c r="L80" s="65"/>
+      <c r="M80" s="65"/>
+      <c r="N80" s="65"/>
+      <c r="O80" s="65"/>
+      <c r="P80" s="65"/>
+      <c r="Q80" s="65"/>
       <c r="T80" s="7"/>
       <c r="U80" s="8">
         <f>SUM(U77:U79)</f>
@@ -3732,7 +3763,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>33</v>
       </c>
@@ -3746,24 +3777,24 @@
       <c r="E81" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F81" s="64" t="s">
+      <c r="F81" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="G81" s="64"/>
-      <c r="H81" s="64"/>
-      <c r="I81" s="61" t="s">
+      <c r="G81" s="66"/>
+      <c r="H81" s="66"/>
+      <c r="I81" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="J81" s="61"/>
-      <c r="K81" s="61"/>
-      <c r="L81" s="60"/>
-      <c r="M81" s="60"/>
-      <c r="N81" s="60"/>
-      <c r="O81" s="60"/>
-      <c r="P81" s="60"/>
-      <c r="Q81" s="60"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J81" s="67"/>
+      <c r="K81" s="67"/>
+      <c r="L81" s="65"/>
+      <c r="M81" s="65"/>
+      <c r="N81" s="65"/>
+      <c r="O81" s="65"/>
+      <c r="P81" s="65"/>
+      <c r="Q81" s="65"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>34</v>
       </c>
@@ -3777,24 +3808,24 @@
       <c r="E82" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F82" s="64" t="s">
+      <c r="F82" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="61" t="s">
+      <c r="G82" s="66"/>
+      <c r="H82" s="66"/>
+      <c r="I82" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J82" s="61"/>
-      <c r="K82" s="61"/>
-      <c r="L82" s="60"/>
-      <c r="M82" s="60"/>
-      <c r="N82" s="60"/>
-      <c r="O82" s="60"/>
-      <c r="P82" s="60"/>
-      <c r="Q82" s="60"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J82" s="67"/>
+      <c r="K82" s="67"/>
+      <c r="L82" s="65"/>
+      <c r="M82" s="65"/>
+      <c r="N82" s="65"/>
+      <c r="O82" s="65"/>
+      <c r="P82" s="65"/>
+      <c r="Q82" s="65"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>35</v>
       </c>
@@ -3808,24 +3839,24 @@
       <c r="E83" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F83" s="64" t="s">
+      <c r="F83" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="61" t="s">
+      <c r="G83" s="66"/>
+      <c r="H83" s="66"/>
+      <c r="I83" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="J83" s="61"/>
-      <c r="K83" s="61"/>
-      <c r="L83" s="60"/>
-      <c r="M83" s="60"/>
-      <c r="N83" s="60"/>
-      <c r="O83" s="60"/>
-      <c r="P83" s="60"/>
-      <c r="Q83" s="60"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J83" s="67"/>
+      <c r="K83" s="67"/>
+      <c r="L83" s="65"/>
+      <c r="M83" s="65"/>
+      <c r="N83" s="65"/>
+      <c r="O83" s="65"/>
+      <c r="P83" s="65"/>
+      <c r="Q83" s="65"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>32</v>
       </c>
@@ -3839,24 +3870,24 @@
       <c r="E84" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="F84" s="64" t="s">
+      <c r="F84" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="G84" s="64"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="61" t="s">
+      <c r="G84" s="66"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="J84" s="61"/>
-      <c r="K84" s="61"/>
-      <c r="L84" s="60"/>
-      <c r="M84" s="60"/>
-      <c r="N84" s="60"/>
-      <c r="O84" s="60"/>
-      <c r="P84" s="60"/>
-      <c r="Q84" s="60"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J84" s="67"/>
+      <c r="K84" s="67"/>
+      <c r="L84" s="65"/>
+      <c r="M84" s="65"/>
+      <c r="N84" s="65"/>
+      <c r="O84" s="65"/>
+      <c r="P84" s="65"/>
+      <c r="Q84" s="65"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="8">
         <f>SUM(B77:B84)</f>
@@ -3866,9 +3897,758 @@
         <f t="shared" si="24"/>
         <v>180</v>
       </c>
+      <c r="E85" s="46"/>
+      <c r="F85" s="46"/>
+      <c r="G85" s="46"/>
+      <c r="H85" s="46"/>
+      <c r="I85" s="46"/>
+      <c r="J85" s="46"/>
+      <c r="K85" s="46"/>
+      <c r="L85" s="46"/>
+      <c r="M85" s="46"/>
+      <c r="N85" s="46"/>
+      <c r="O85" s="46"/>
+      <c r="P85" s="46"/>
+      <c r="Q85" s="46"/>
+      <c r="R85" s="46"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="C87" s="61"/>
+    </row>
+    <row r="88" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="61">
+        <v>5</v>
+      </c>
+      <c r="V88" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="W88" s="60"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E89" s="38"/>
+      <c r="F89" s="40">
+        <v>1</v>
+      </c>
+      <c r="G89" s="41">
+        <v>2</v>
+      </c>
+      <c r="H89" s="42">
+        <v>3</v>
+      </c>
+      <c r="I89" s="40">
+        <v>4</v>
+      </c>
+      <c r="J89" s="41">
+        <v>5</v>
+      </c>
+      <c r="K89" s="42">
+        <v>6</v>
+      </c>
+      <c r="L89" s="40">
+        <v>7</v>
+      </c>
+      <c r="M89" s="41">
+        <v>8</v>
+      </c>
+      <c r="N89" s="42">
+        <v>9</v>
+      </c>
+      <c r="O89" s="40">
+        <v>10</v>
+      </c>
+      <c r="P89" s="41">
+        <v>11</v>
+      </c>
+      <c r="Q89" s="42">
+        <v>12</v>
+      </c>
+      <c r="T89" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V89" s="3">
+        <v>20</v>
+      </c>
+      <c r="X89" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y89" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z89" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="5">
+        <v>1</v>
+      </c>
+      <c r="C90" s="62">
+        <f>B90*$C$88</f>
+        <v>5</v>
+      </c>
+      <c r="E90" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F90" s="66">
+        <v>1</v>
+      </c>
+      <c r="G90" s="66"/>
+      <c r="H90" s="66"/>
+      <c r="I90" s="67">
+        <v>1</v>
+      </c>
+      <c r="J90" s="67"/>
+      <c r="K90" s="67"/>
+      <c r="L90" s="65"/>
+      <c r="M90" s="65"/>
+      <c r="N90" s="65"/>
+      <c r="O90" s="65"/>
+      <c r="P90" s="65"/>
+      <c r="Q90" s="65"/>
+      <c r="R90" s="25">
+        <v>42248</v>
+      </c>
+      <c r="T90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U90" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="V90" s="6">
+        <f>U90*$V$89</f>
+        <v>10</v>
+      </c>
+      <c r="X90" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y90" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z90" s="6">
+        <f>Y90*$Z$89</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91" s="8">
+        <v>1</v>
+      </c>
+      <c r="C91" s="63">
+        <f>B91*$C$88</f>
+        <v>5</v>
+      </c>
+      <c r="E91" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91" s="66">
+        <v>2</v>
+      </c>
+      <c r="G91" s="66"/>
+      <c r="H91" s="66"/>
+      <c r="I91" s="67">
+        <v>2</v>
+      </c>
+      <c r="J91" s="67"/>
+      <c r="K91" s="67"/>
+      <c r="L91" s="65"/>
+      <c r="M91" s="65"/>
+      <c r="N91" s="65"/>
+      <c r="O91" s="65"/>
+      <c r="P91" s="65"/>
+      <c r="Q91" s="65"/>
+      <c r="R91" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="T91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U91" s="5">
+        <v>5</v>
+      </c>
+      <c r="V91" s="6">
+        <f t="shared" ref="V91:V93" si="26">U91*$V$89</f>
+        <v>100</v>
+      </c>
+      <c r="X91" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y91" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z91" s="6">
+        <f t="shared" ref="Z91:Z92" si="27">Y91*$Z$89</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A92" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="62"/>
+      <c r="E92" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="66">
+        <v>3</v>
+      </c>
+      <c r="G92" s="66"/>
+      <c r="H92" s="66"/>
+      <c r="I92" s="67">
+        <v>3</v>
+      </c>
+      <c r="J92" s="67"/>
+      <c r="K92" s="67"/>
+      <c r="L92" s="65"/>
+      <c r="M92" s="65"/>
+      <c r="N92" s="65"/>
+      <c r="O92" s="65"/>
+      <c r="P92" s="65"/>
+      <c r="Q92" s="65"/>
+      <c r="R92" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="T92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U92" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="V92" s="6">
+        <f t="shared" si="26"/>
+        <v>50</v>
+      </c>
+      <c r="X92" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y92" s="8">
+        <v>10</v>
+      </c>
+      <c r="Z92" s="9">
+        <f t="shared" si="27"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93" s="2">
+        <v>4</v>
+      </c>
+      <c r="C93" s="61">
+        <f t="shared" ref="C93:C98" si="28">B93*$C$88</f>
+        <v>20</v>
+      </c>
+      <c r="E93" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F93" s="66">
+        <v>4</v>
+      </c>
+      <c r="G93" s="66"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="67">
+        <v>4</v>
+      </c>
+      <c r="J93" s="67"/>
+      <c r="K93" s="67"/>
+      <c r="L93" s="65"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
+      <c r="O93" s="65"/>
+      <c r="P93" s="65"/>
+      <c r="Q93" s="65"/>
+      <c r="T93" s="7"/>
+      <c r="U93" s="8">
+        <f>SUM(U90:U92)</f>
+        <v>8</v>
+      </c>
+      <c r="V93" s="6">
+        <f t="shared" si="26"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B94" s="5">
+        <v>2</v>
+      </c>
+      <c r="C94" s="62">
+        <f t="shared" si="28"/>
+        <v>10</v>
+      </c>
+      <c r="E94" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G94" s="66"/>
+      <c r="H94" s="66"/>
+      <c r="I94" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="J94" s="67"/>
+      <c r="K94" s="67"/>
+      <c r="L94" s="65"/>
+      <c r="M94" s="65"/>
+      <c r="N94" s="65"/>
+      <c r="O94" s="65"/>
+      <c r="P94" s="65"/>
+      <c r="Q94" s="65"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B95" s="5">
+        <v>1</v>
+      </c>
+      <c r="C95" s="62">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="E95" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="65"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="65"/>
+      <c r="L95" s="65"/>
+      <c r="M95" s="65"/>
+      <c r="N95" s="65"/>
+      <c r="O95" s="65"/>
+      <c r="P95" s="65"/>
+      <c r="Q95" s="65"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C96" s="62">
+        <f t="shared" si="28"/>
+        <v>2.5</v>
+      </c>
+      <c r="E96" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="65"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
+      <c r="J96" s="65"/>
+      <c r="K96" s="65"/>
+      <c r="L96" s="65"/>
+      <c r="M96" s="65"/>
+      <c r="N96" s="65"/>
+      <c r="O96" s="65"/>
+      <c r="P96" s="65"/>
+      <c r="Q96" s="65"/>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97" s="8">
+        <v>1</v>
+      </c>
+      <c r="C97" s="63">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="E97" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F97" s="65"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="65"/>
+      <c r="I97" s="65"/>
+      <c r="J97" s="65"/>
+      <c r="K97" s="65"/>
+      <c r="L97" s="65"/>
+      <c r="M97" s="65"/>
+      <c r="N97" s="65"/>
+      <c r="O97" s="65"/>
+      <c r="P97" s="65"/>
+      <c r="Q97" s="65"/>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A98" s="7"/>
+      <c r="B98" s="8">
+        <f>SUM(B87:B97)</f>
+        <v>20</v>
+      </c>
+      <c r="C98" s="62">
+        <f t="shared" si="28"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E100" s="38"/>
+      <c r="F100" s="40">
+        <v>1</v>
+      </c>
+      <c r="G100" s="41">
+        <v>2</v>
+      </c>
+      <c r="H100" s="42">
+        <v>3</v>
+      </c>
+      <c r="I100" s="40">
+        <v>4</v>
+      </c>
+      <c r="J100" s="41">
+        <v>5</v>
+      </c>
+      <c r="K100" s="42">
+        <v>6</v>
+      </c>
+      <c r="L100" s="40">
+        <v>7</v>
+      </c>
+      <c r="M100" s="41">
+        <v>8</v>
+      </c>
+      <c r="N100" s="42">
+        <v>9</v>
+      </c>
+      <c r="O100" s="40">
+        <v>10</v>
+      </c>
+      <c r="P100" s="41">
+        <v>11</v>
+      </c>
+      <c r="Q100" s="42">
+        <v>12</v>
+      </c>
+      <c r="T100" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U100" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V100" s="3">
+        <f>13*3*1.2</f>
+        <v>46.8</v>
+      </c>
+      <c r="X100" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y100" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z100" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C101" s="25">
+        <v>42265</v>
+      </c>
+      <c r="E101" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F101" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="G101" s="66"/>
+      <c r="H101" s="66"/>
+      <c r="I101" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="J101" s="66"/>
+      <c r="K101" s="66"/>
+      <c r="L101" s="65"/>
+      <c r="M101" s="65"/>
+      <c r="N101" s="65"/>
+      <c r="O101" s="65"/>
+      <c r="P101" s="65"/>
+      <c r="Q101" s="65"/>
+      <c r="R101" s="25">
+        <v>42248</v>
+      </c>
+      <c r="T101" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U101" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="V101" s="6">
+        <f>U101*$V$100</f>
+        <v>23.4</v>
+      </c>
+      <c r="X101" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y101" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z101" s="6">
+        <f>Y101*$Z$76</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E102" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F102" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G102" s="66"/>
+      <c r="H102" s="66"/>
+      <c r="I102" s="66">
+        <v>5</v>
+      </c>
+      <c r="J102" s="66"/>
+      <c r="K102" s="66"/>
+      <c r="L102" s="65"/>
+      <c r="M102" s="65"/>
+      <c r="N102" s="65"/>
+      <c r="O102" s="65"/>
+      <c r="P102" s="65"/>
+      <c r="Q102" s="65"/>
+      <c r="R102" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="T102" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U102" s="5">
+        <v>5</v>
+      </c>
+      <c r="V102" s="6">
+        <f t="shared" ref="V102:V104" si="29">U102*$V$100</f>
+        <v>234</v>
+      </c>
+      <c r="X102" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y102" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z102" s="6">
+        <f>Y102*$Z$76</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E103" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="G103" s="66"/>
+      <c r="H103" s="66"/>
+      <c r="I103" s="66">
+        <v>6</v>
+      </c>
+      <c r="J103" s="66"/>
+      <c r="K103" s="66"/>
+      <c r="L103" s="65"/>
+      <c r="M103" s="65"/>
+      <c r="N103" s="65"/>
+      <c r="O103" s="65"/>
+      <c r="P103" s="65"/>
+      <c r="Q103" s="65"/>
+      <c r="R103" t="s">
+        <v>68</v>
+      </c>
+      <c r="T103" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U103" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="V103" s="6">
+        <f t="shared" si="29"/>
+        <v>117</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y103" s="8">
+        <v>10</v>
+      </c>
+      <c r="Z103" s="6">
+        <f>Y103*$Z$76</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E104" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="G104" s="66"/>
+      <c r="H104" s="66"/>
+      <c r="I104" s="66">
+        <v>7</v>
+      </c>
+      <c r="J104" s="66"/>
+      <c r="K104" s="66"/>
+      <c r="L104" s="65"/>
+      <c r="M104" s="65"/>
+      <c r="N104" s="65"/>
+      <c r="O104" s="65"/>
+      <c r="P104" s="65"/>
+      <c r="Q104" s="65"/>
+      <c r="R104" t="s">
+        <v>69</v>
+      </c>
+      <c r="T104" s="7"/>
+      <c r="U104" s="8">
+        <f>SUM(U101:U103)</f>
+        <v>8</v>
+      </c>
+      <c r="V104" s="6">
+        <f t="shared" si="29"/>
+        <v>374.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E105" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="G105" s="66"/>
+      <c r="H105" s="66"/>
+      <c r="I105" s="66">
+        <v>8</v>
+      </c>
+      <c r="J105" s="66"/>
+      <c r="K105" s="66"/>
+      <c r="L105" s="65"/>
+      <c r="M105" s="65"/>
+      <c r="N105" s="65"/>
+      <c r="O105" s="65"/>
+      <c r="P105" s="65"/>
+      <c r="Q105" s="65"/>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E106" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="G106" s="66"/>
+      <c r="H106" s="66"/>
+      <c r="I106" s="65"/>
+      <c r="J106" s="65"/>
+      <c r="K106" s="65"/>
+      <c r="L106" s="65"/>
+      <c r="M106" s="65"/>
+      <c r="N106" s="65"/>
+      <c r="O106" s="65"/>
+      <c r="P106" s="65"/>
+      <c r="Q106" s="65"/>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E107" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="G107" s="66"/>
+      <c r="H107" s="66"/>
+      <c r="I107" s="65"/>
+      <c r="J107" s="65"/>
+      <c r="K107" s="65"/>
+      <c r="L107" s="65"/>
+      <c r="M107" s="65"/>
+      <c r="N107" s="65"/>
+      <c r="O107" s="65"/>
+      <c r="P107" s="65"/>
+      <c r="Q107" s="65"/>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E108" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F108" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="G108" s="66"/>
+      <c r="H108" s="66"/>
+      <c r="I108" s="65"/>
+      <c r="J108" s="65"/>
+      <c r="K108" s="65"/>
+      <c r="L108" s="65"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="65"/>
+      <c r="O108" s="65"/>
+      <c r="P108" s="65"/>
+      <c r="Q108" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="237">
+  <mergeCells count="301">
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I107:K107"/>
+    <mergeCell ref="L107:N107"/>
+    <mergeCell ref="O107:Q107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="I108:K108"/>
+    <mergeCell ref="L108:N108"/>
+    <mergeCell ref="O108:Q108"/>
+    <mergeCell ref="L101:N101"/>
+    <mergeCell ref="L102:N102"/>
+    <mergeCell ref="L103:N103"/>
+    <mergeCell ref="L104:N104"/>
+    <mergeCell ref="L105:N105"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="I104:K104"/>
+    <mergeCell ref="O104:Q104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="I105:K105"/>
+    <mergeCell ref="O105:Q105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="I106:K106"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="O106:Q106"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="I101:K101"/>
+    <mergeCell ref="O101:Q101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="I102:K102"/>
+    <mergeCell ref="O102:Q102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="I103:K103"/>
+    <mergeCell ref="O103:Q103"/>
     <mergeCell ref="F83:H83"/>
     <mergeCell ref="I83:K83"/>
     <mergeCell ref="L83:N83"/>
@@ -3982,8 +4762,6 @@
     <mergeCell ref="L51:N51"/>
     <mergeCell ref="F50:H50"/>
     <mergeCell ref="I50:K50"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="I37:K37"/>
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="I47:K47"/>
     <mergeCell ref="F38:H38"/>
@@ -4006,6 +4784,8 @@
     <mergeCell ref="L43:N43"/>
     <mergeCell ref="F40:H40"/>
     <mergeCell ref="I40:K40"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="I37:K37"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:K30"/>
     <mergeCell ref="L30:N30"/>
@@ -4106,8 +4886,40 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I4:K4"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="I90:K90"/>
+    <mergeCell ref="L90:N90"/>
+    <mergeCell ref="O90:Q90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="I91:K91"/>
+    <mergeCell ref="L91:N91"/>
+    <mergeCell ref="O91:Q91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="I92:K92"/>
+    <mergeCell ref="L92:N92"/>
+    <mergeCell ref="O92:Q92"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="I96:K96"/>
+    <mergeCell ref="L96:N96"/>
+    <mergeCell ref="O96:Q96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="I97:K97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="O97:Q97"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="I93:K93"/>
+    <mergeCell ref="L93:N93"/>
+    <mergeCell ref="O93:Q93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="I94:K94"/>
+    <mergeCell ref="L94:N94"/>
+    <mergeCell ref="O94:Q94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="O95:Q95"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>